<commit_message>
updated create TI and TS
</commit_message>
<xml_diff>
--- a/STUDY001_TI.xlsx
+++ b/STUDY001_TI.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t xml:space="preserve">STUDYID</t>
   </si>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">INCL1</t>
   </si>
   <si>
-    <t xml:space="preserve">Inclusion Criteria Patients must meet the following criteria for study entry:</t>
+    <t xml:space="preserve">Inclusion Criteria All patients and subjects will be willing to commit to training and data collection that includes video recording, which may be used for educational and (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">INCLUSION</t>
@@ -56,103 +56,103 @@
     <t xml:space="preserve">INCL2</t>
   </si>
   <si>
-    <t xml:space="preserve">Signed Informed Consent Form</t>
+    <t xml:space="preserve">Able to give informed consent and willing to comply with the requirements of the study protocol</t>
   </si>
   <si>
     <t xml:space="preserve">INCL3</t>
   </si>
   <si>
-    <t xml:space="preserve">Age ≥ 18 years at time of signing Informed Consent Form</t>
+    <t xml:space="preserve">Age ≥ 18 years</t>
   </si>
   <si>
     <t xml:space="preserve">INCL4</t>
   </si>
   <si>
-    <t xml:space="preserve">Ability to comply with the study protocol, including willingness to remain in the post-treatment period</t>
+    <t xml:space="preserve">Be a current resident within the United States</t>
   </si>
   <si>
     <t xml:space="preserve">INCL5</t>
   </si>
   <si>
-    <t xml:space="preserve">ECOG Performance Status of 0 or 1 (see Appendix 3)</t>
+    <t xml:space="preserve">Have had RA for ≥ 6 months, as diagnosed by a qualiﬁed rheumatologist, according to the revised 1987 American College of Rheumatology (ACR) criteria (Arnett et al. 1988)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL6</t>
   </si>
   <si>
-    <t xml:space="preserve">Histologically or cytologically documented NSCLC with unresectable Stage III NSCLC of either squamous or non-squamous histology Staging should be based on the 8th revised (As per the protocol)</t>
+    <t xml:space="preserve">Patients must be deemed suitable candidates to use an AI at home, in the investigator’s judgment, either by self-administration or from a CG or from a HCP</t>
   </si>
   <si>
     <t xml:space="preserve">INCL7</t>
   </si>
   <si>
-    <t xml:space="preserve">Whole-body positron emission tomography (PET)-CT scan (from the base of skull to mid-thighs) for the purposes of staging, performed prior and within 42 days of the first dose of (As per the protocol)</t>
+    <t xml:space="preserve">Have been receiving 162 mg TCZ SC q2w or qw using the commercially Molecule Name and Protocol Name – Organization Name 6 / Protocol XX12346, Version 2.1 available PFS-NSD for at (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL8</t>
   </si>
   <si>
-    <t xml:space="preserve">The RT component in the CRT must have been at a total dose of radiation of 60 (± 10) Gy (54−66 Gy) administered by IMRT (preferred) or 3D-conforming technique Sites are (As per the protocol)</t>
+    <t xml:space="preserve">Most recent laboratory results performed in accordance with the current Actemra U.S. Prescribing Information (USPI) do not warrant dose adjustment or discontinuation of therapy (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL9</t>
   </si>
   <si>
-    <t xml:space="preserve">No progression during or following concurrent platinum-based CRT</t>
+    <t xml:space="preserve">At least 2 self-injecting patients will be left-hand dominant</t>
   </si>
   <si>
     <t xml:space="preserve">INCL10</t>
   </si>
   <si>
-    <t xml:space="preserve">Tumor PD-L1 expression, as determined by SP263 IHC assay and documented by means of central testing of a representative tumor tissue, in either a previously obtained archival (As per the protocol)</t>
+    <t xml:space="preserve">To continue using contraception as discussed with the patient’s rheumatologist at the time of prescription of TCZ SC PFS-NSD 4.1.1.2 Caregivers CGs may be already acquainted (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL11</t>
   </si>
   <si>
-    <t xml:space="preserve">Confirmed availability of representative tumor specimens in formalin- fixed, paraffin-embedded (FFPE) blocks (preferred) or at least 15−20 unstained serial slides, along with an (As per the protocol)</t>
-  </si>
-  <si>
     <t xml:space="preserve">INCL12</t>
   </si>
   <si>
-    <t xml:space="preserve">Life expectancy ≥ 12 weeks</t>
-  </si>
-  <si>
     <t xml:space="preserve">INCL13</t>
   </si>
   <si>
-    <t xml:space="preserve">Negative HIV test at screening</t>
+    <t xml:space="preserve">Not professionally qualiﬁed to give an injection (e.g., a patient’s spouse, relative).</t>
   </si>
   <si>
     <t xml:space="preserve">INCL14</t>
   </si>
   <si>
-    <t xml:space="preserve">Negative hepatitis B surface antigen (HBsAg) test at screening</t>
+    <t xml:space="preserve">Able (after training) and willing to inject a patient at each visit</t>
   </si>
   <si>
     <t xml:space="preserve">INCL15</t>
   </si>
   <si>
-    <t xml:space="preserve">Positive hepatitis B surface antibody (HBsAb) test at screening, or negative HBsAb at screening accompanied by either of the following: – Negative hepatitis B core antibody (As per the protocol)</t>
+    <t xml:space="preserve">Must be current resident within the United States 4.1.1.3 Healthcare Professionals An HCP may be already acquainted with (and already supporting) a specific patient enrolled in (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL16</t>
   </si>
   <si>
-    <t xml:space="preserve">For women of childbearing potential: agreement to remain abstinent (refrain from heterosexual intercourse) or use contraception, and agreement to refrain from donating eggs, as (As per the protocol)</t>
-  </si>
-  <si>
     <t xml:space="preserve">INCL17</t>
   </si>
   <si>
-    <t xml:space="preserve">For men: agreement to remain abstinent (refrain from heterosexual intercourse) or use a condom, and agreement to refrain from donating sperm, as defined below: With a female (As per the protocol)</t>
+    <t xml:space="preserve">INCL18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must be current resident of the United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INCL19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professionally qualiﬁed to give an injection and willing to inject a patient and comply with the study protocol</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL1</t>
   </si>
   <si>
-    <t xml:space="preserve">Exclusion Criteria Patients who meet any of the following criteria will be excluded from study entry:</t>
+    <t xml:space="preserve">Exclusion Criteria 4.1.2.1 Patients Patients who meet any of the following criteria will be excluded from study entry:</t>
   </si>
   <si>
     <t xml:space="preserve">EXCLUSION</t>
@@ -161,187 +161,136 @@
     <t xml:space="preserve">EXCL2</t>
   </si>
   <si>
-    <t xml:space="preserve">NSCLC known to have a mutation in the EGFR gene or an ALK fusion oncogene are excluded from the study: – Patients with non-squamous NSCLC who have an unknown EGFR or ALK status (As per the protocol)</t>
+    <t xml:space="preserve">Any serious medical condition or abnormality in clinical laboratory tests that, in the investigator’s judgment, precludes the patient’s safe participation Molecule Name and (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL3</t>
   </si>
   <si>
-    <t xml:space="preserve">If a pleural effusion is present, the following criteria must be met to exclude malignant involvement (incurable T4 disease): – When pleural fluid is visible on both the (As per the protocol)</t>
+    <t xml:space="preserve">Patients with functional RA status class IV (according to the 1991 ACR revised criteria for the classiﬁcation of global functional status in RA [Hochberg et al. 1992]), as (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL4</t>
   </si>
   <si>
-    <t xml:space="preserve">Any evidence of Stage IV disease, including, but not limited to, the following: – Pleural effusion – Pericardial effusion – Brain metastases – No history of intracranial (As per the protocol)</t>
+    <t xml:space="preserve">Neuropathies or other conditions that might interfere with pain evaluation</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL5</t>
   </si>
   <si>
-    <t xml:space="preserve">Pulmonary lymphoepithelioma-like carcinoma subtype of NSCLC</t>
+    <t xml:space="preserve">Current participation in any interventional clinical trial</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL6</t>
   </si>
   <si>
-    <t xml:space="preserve">History of leptomeningeal disease</t>
+    <t xml:space="preserve">Patients who self-report to be pregnant or nursing (breastfeeding)</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL7</t>
   </si>
   <si>
-    <t xml:space="preserve">Concurrent enrollment in another clinical study, unless it is an observational (non- interventional) clinical study or the follow-up period of an interventional study</t>
+    <t xml:space="preserve">Patient or anyone in his/her immediate household is employed in the pharmaceutical industry</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL8</t>
   </si>
   <si>
-    <t xml:space="preserve">Treatment with sequential CRT for locally advanced NSCLC</t>
+    <t xml:space="preserve">Patient employed by Roche, Genentech, Battelle, or a contract research organization (CRO) involved in this study (WA29917)</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL9</t>
   </si>
   <si>
-    <t xml:space="preserve">Patients with locally advanced NSCLC who have progressed during or after the definite concurrent CRT prior to randomization</t>
+    <t xml:space="preserve">Participation in any previous Actemra research study that involved an AI.</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL10</t>
   </si>
   <si>
-    <t xml:space="preserve">Grade ≥ 2 pneumonitis from prior CRT</t>
+    <t xml:space="preserve">Prior use of the AI-1000 G1 or AI-1000 G2 in any HF study.</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL11</t>
   </si>
   <si>
-    <t xml:space="preserve">Any concurrent chemotherapy, immunotherapy, biologic, or hormonal therapy for cancer Note: Local treatment of isolated lesions, excluding target lesions, with palliative intent (As per the protocol)</t>
+    <t xml:space="preserve">ANC &lt; 1.0 × 109/L (1000/mm3) at last (as per the USPI) laboratory assessment.</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL12</t>
   </si>
   <si>
-    <t xml:space="preserve">Uncontrolled or symptomatic hypercalcemia (ionized calcium &gt; 1.5 mmol/L, calcium &gt; 12 mg/dL, or corrected calcium greater than ULN)</t>
+    <t xml:space="preserve">Platelet count &lt; 100 × 109/L (100,000/mm3) at last laboratory assessment.</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL13</t>
   </si>
   <si>
-    <t xml:space="preserve">Active or history of autoimmune disease or immune deficiency, including, but not limited to, myasthenia gravis, myositis, autoimmune hepatitis, systemic lupus erythematosus, (As per the protocol)</t>
+    <t xml:space="preserve">ALT or AST &gt; upper limit of normal [ULN] at last laboratory assessment. 4.1.2.2 Caregivers CGs who meet any of the following criteria will be excluded from study entry:</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL14</t>
   </si>
   <si>
-    <t xml:space="preserve">History of idiopathic pulmonary fibrosis, organizing pneumonia (e.g., bronchiolitis obliterans), drug-induced pneumonitis, or idiopathic pneumonitis, or evidence of active (As per the protocol)</t>
-  </si>
-  <si>
     <t xml:space="preserve">EXCL15</t>
   </si>
   <si>
-    <t xml:space="preserve">Known clinically significant liver disease, including active viral, alcoholic, or other hepatitis, cirrhosis, and inherited liver disease, or current alcohol abuse</t>
+    <t xml:space="preserve">Subject or anyone in his/her immediate household is employed in the pharmaceutical industry</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL16</t>
   </si>
   <si>
-    <t xml:space="preserve">Significant cardiovascular disease (such as New York Heart Association Class II or greater cardiac disease, myocardial infarction, or cerebrovascular accident) within 3 months (As per the protocol)</t>
+    <t xml:space="preserve">Subject employed by Roche, Genentech, Battelle, or a CRO involved in this study (WA29917) 4.1.2.3 Healthcare Professionals HCPs who meet any of the following criteria will be (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL17</t>
   </si>
   <si>
-    <t xml:space="preserve">Major surgical procedure, other than for diagnosis, within 4 weeks prior to initiation of study treatment, or anticipation of need for a major surgical procedure during the study</t>
+    <t xml:space="preserve">Current participation in any interventional clinical trial as a patient</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL18</t>
   </si>
   <si>
-    <t xml:space="preserve">History of malignancy other than NSCLC within 5 years prior to screening, with the exception of malignancies with a negligible risk of metastasis or death (e.g., 5-year OS rate (As per the protocol)</t>
+    <t xml:space="preserve">Participation in the conduct or oversight of this study (WA29917)</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL19</t>
   </si>
   <si>
-    <t xml:space="preserve">Severe infection within 4 weeks prior to initiation of study treatment, including, but not limited to, hospitalization for complications of infection, bacteremia, or severe (As per the protocol)</t>
+    <t xml:space="preserve">Subject or anyone in his/her immediate household is employed in the pharmaceutical industry.</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL20</t>
   </si>
   <si>
-    <t xml:space="preserve">Treatment with therapeutic oral or IV antibiotics within 2 weeks prior to initiation of study treatment Patients receiving prophylactic antibiotics (e.g., to prevent a urinary (As per the protocol)</t>
+    <t xml:space="preserve">Subject employed by Roche, Genentech, Battelle or a CRO involved in this study (WA29917) Molecule Name and Protocol Name – Organization Name 8 / Protocol XX12346, Version 2.1</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL21</t>
   </si>
   <si>
-    <t xml:space="preserve">Prior allogeneic stem cell or solid organ transplantation</t>
+    <t xml:space="preserve">Not professionally qualiﬁed to give injections 4.2 METHOD OF TREATMENT ASSIGNMENT AND BLINDING Patients will take part in the study in one of three groups:</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL22</t>
   </si>
   <si>
-    <t xml:space="preserve">Any other disease, metabolic dysfunction, physical examination finding, or clinical laboratory finding that contraindicates the use of an investigational drug, may affect the (As per the protocol)</t>
+    <t xml:space="preserve">Self-injecting patients</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL23</t>
   </si>
   <si>
-    <t xml:space="preserve">Treatment with a live, attenuated vaccine within 4 weeks prior to initiation of study treatment, or anticipation of need for such a vaccine during study treatment or within 5 (As per the protocol)</t>
+    <t xml:space="preserve">Patients who receive injections from a CG</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL24</t>
   </si>
   <si>
-    <t xml:space="preserve">Current treatment with anti-viral therapy for HBV or HCV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXCL25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment with investigational therapy within 28 days prior to initiation of study treatment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXCL26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prior treatment with CD137 agonists or immune checkpoint blockade therapies, including anti−cytotoxic T lymphocyte−associated protein 4, anti-TIGIT, anti−PD-1, and anti−PD-L1 (As per the protocol)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXCL27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any prior Grade ≥ 3 immune-mediated adverse event or any unresolved Grade &gt; 1 immune-mediated adverse event while receiving any previous immunotherapy agent other than immune (As per the protocol)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXCL28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment with systemic immunostimulatory agents (including, but not limited to, IFN and interleukin-2 [IL-2]) within 4 weeks or 5 drug- elimination half-lives (whichever is (As per the protocol)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXCL29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment with systemic immunosuppressive medication (including, but not limited to, corticosteroids, cyclophosphamide, azathioprine, methotrexate, thalidomide, and anti−tumor (As per the protocol)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXCL30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">History of severe allergic anaphylactic reactions to chimeric or humanized antibodies or fusion proteins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXCL31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Known hypersensitivity to CHO cell products or to any component of the tiragolumab or atezolizumab or durvalumab formulation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXCL32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pregnancy or breastfeeding, or intention of becoming pregnant during study treatment or within 5 months after the final dose of study treatment Women of childbearing potential (As per the protocol)</t>
+    <t xml:space="preserve">Patients who receive injections from an HCP A minimum of 15 patients and/or subjects are required per group, and patients may be assigned so that all groups have the required (As per the protocol)</t>
   </si>
 </sst>
 </file>
@@ -941,7 +890,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
@@ -960,10 +909,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
@@ -982,10 +931,10 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>12</v>
@@ -1004,10 +953,10 @@
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>12</v>
@@ -1026,10 +975,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>12</v>
@@ -1048,10 +997,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>12</v>
@@ -1070,10 +1019,10 @@
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>12</v>
@@ -1092,13 +1041,13 @@
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1114,13 +1063,13 @@
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1136,10 +1085,10 @@
         <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>47</v>
@@ -1158,10 +1107,10 @@
         <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>47</v>
@@ -1180,10 +1129,10 @@
         <v>9</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>47</v>
@@ -1202,10 +1151,10 @@
         <v>9</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>47</v>
@@ -1224,10 +1173,10 @@
         <v>9</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>47</v>
@@ -1246,10 +1195,10 @@
         <v>9</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>47</v>
@@ -1268,10 +1217,10 @@
         <v>9</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>47</v>
@@ -1290,10 +1239,10 @@
         <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>47</v>
@@ -1312,10 +1261,10 @@
         <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>47</v>
@@ -1334,10 +1283,10 @@
         <v>9</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>47</v>
@@ -1356,10 +1305,10 @@
         <v>9</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>47</v>
@@ -1378,10 +1327,10 @@
         <v>9</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>47</v>
@@ -1400,10 +1349,10 @@
         <v>9</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>47</v>
@@ -1422,10 +1371,10 @@
         <v>9</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>47</v>
@@ -1444,10 +1393,10 @@
         <v>9</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>47</v>
@@ -1466,10 +1415,10 @@
         <v>9</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>47</v>
@@ -1488,10 +1437,10 @@
         <v>9</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>47</v>
@@ -1510,10 +1459,10 @@
         <v>9</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>47</v>
@@ -1532,10 +1481,10 @@
         <v>9</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>47</v>
@@ -1554,10 +1503,10 @@
         <v>9</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>47</v>
@@ -1576,10 +1525,10 @@
         <v>9</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>47</v>
@@ -1598,10 +1547,10 @@
         <v>9</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>47</v>
@@ -1620,10 +1569,10 @@
         <v>9</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>47</v>
@@ -1642,10 +1591,10 @@
         <v>9</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>47</v>
@@ -1653,138 +1602,6 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve footnote detection and criteria extraction in PDF parsing
- Enhanced footnote detection to identify multi-line footnotes
- Updated criteria extraction to exclude section headers and introductory text
- Refined page number removal from extracted criteria
- Improved handling of protocol version information in footnotes
- Added more robust error handling and debugging information
</commit_message>
<xml_diff>
--- a/STUDY001_TI.xlsx
+++ b/STUDY001_TI.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t xml:space="preserve">STUDYID</t>
   </si>
@@ -50,96 +50,78 @@
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">Patients must meet the following criteria for study entry: NA</t>
+    <t xml:space="preserve">HER2-positive breast cancer HER2-positive status will be based on pretreatment biopsy material and defined as an immunohistochemistry (IHC) (Appendix 6) score of 3+ and/or posit... (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL002</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.1 Disease-Specific Inclusion Criteria</t>
+    <t xml:space="preserve">Histologically confirmed invasive breast carcinoma</t>
   </si>
   <si>
     <t xml:space="preserve">INCL003</t>
   </si>
   <si>
-    <t xml:space="preserve">HER2-positive breast cancer HER2-positive status will be based on pretreatment biopsy material and defined as an immunohistochemistry (IHC) (Appendix 6) score of 3+ and/or posit... (As per the protocol)</t>
+    <t xml:space="preserve">Clinical stage at presentation: T1–4, N0–3, M0 (Note: Patients with T1a/bN0 tumors will not be eligible)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL004</t>
   </si>
   <si>
-    <t xml:space="preserve">Histologically confirmed invasive breast carcinoma</t>
+    <t xml:space="preserve">Completion of preoperative systemic chemotherapy and HER2-directed treatment. Systemic therapy must consist of at least 6 cycles of chemotherapy, with a total duration at least... (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL005</t>
   </si>
   <si>
-    <t xml:space="preserve">Clinical stage at presentation: T1–4, N0–3, M0 (Note: Patients with T1a/bN0 tumors will not be eligible)</t>
+    <t xml:space="preserve">Adequate excision: surgical removal of all clinically evident disease in the breast and lymph nodes as follows: Breast surgery: total mastectomy with no gross residual disease a... (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL006</t>
   </si>
   <si>
-    <t xml:space="preserve">Completion of preoperative systemic chemotherapy and HER2-directed treatment. Systemic therapy must consist of at least 6 cycles of chemotherapy, with a total duration at least... (As per the protocol)</t>
+    <t xml:space="preserve">Pathologic evidence of residual invasive carcinoma in the breast or axillary lymph nodes following completion of preoperative therapy. If invasive disease is present in both bre... (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL007</t>
   </si>
   <si>
-    <t xml:space="preserve">Adequate excision: surgical removal of all clinically evident disease in the breast and lymph nodes as follows: Breast surgery: total mastectomy with no gross residual disease a... (As per the protocol)</t>
+    <t xml:space="preserve">An interval of no more than 12 weeks between the date of primary surgery and the date of randomization</t>
   </si>
   <si>
     <t xml:space="preserve">INCL008</t>
   </si>
   <si>
-    <t xml:space="preserve">Pathologic evidence of residual invasive carcinoma in the breast or axillary lymph nodes following completion of preoperative therapy. If invasive disease is present in both bre... (As per the protocol)</t>
+    <t xml:space="preserve">Known hormone receptor status Hormone receptor−positive status can be determined by either known positive ER or known positive PgR status; hormone receptor−negative status must... (As per the protocol)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL009</t>
   </si>
   <si>
-    <t xml:space="preserve">An interval of no more than 12 weeks between the date of primary surgery and the date of randomization</t>
+    <t xml:space="preserve">Signed written informed consent approved by the study site’s Institutional Review Board (IRB)/Ethical Committee (EC)</t>
   </si>
   <si>
     <t xml:space="preserve">INCL010</t>
   </si>
   <si>
-    <t xml:space="preserve">Known hormone receptor status Hormone receptor−positive status can be determined by either known positive ER or known positive PgR status; hormone receptor−negative status must... (As per the protocol)</t>
+    <t xml:space="preserve">Age ≥ 18 years</t>
   </si>
   <si>
     <t xml:space="preserve">INCL011</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.2 General Inclusion Criteria</t>
+    <t xml:space="preserve">Eastern Cooperative Oncology Group (ECOG) performance status 0 or 1</t>
   </si>
   <si>
     <t xml:space="preserve">INCL012</t>
   </si>
   <si>
-    <t xml:space="preserve">Signed written informed consent approved by the study site’s Institutional Review Board (IRB)/Ethical Committee (EC)</t>
+    <t xml:space="preserve">Life expectancy ≥ 6 months</t>
   </si>
   <si>
     <t xml:space="preserve">INCL013</t>
   </si>
   <si>
-    <t xml:space="preserve">Age ≥ 18 years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INCL014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Cooperative Oncology Group (ECOG) performance status 0 or 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INCL015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Life expectancy ≥ 6 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INCL016</t>
-  </si>
-  <si>
     <t xml:space="preserve">Adequate organ function during screening, defined as: a. Absolute neutrophil count ≥ 1200 cells/mm3 b. Platelet count ≥ 100000 cells/mm3 c. Hemoglobin ≥ 9.0 g/dL; patients may r... (As per the protocol)</t>
   </si>
   <si>
@@ -149,13 +131,97 @@
     <t xml:space="preserve">Exclusion Criteria</t>
   </si>
   <si>
-    <t xml:space="preserve">Patients who meet any of the following criteria will be excluded from study entry. NA</t>
+    <t xml:space="preserve">Stage IV (metastatic) breast cancer</t>
   </si>
   <si>
     <t xml:space="preserve">EXCL002</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2.1 Disease-Related Exclusion Criteria</t>
+    <t xml:space="preserve">History of any prior (ipsi- or contralateral) breast cancer except lobular CIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evidence of clinically evident gross residual or recurrent disease following preoperative therapy and surgery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An overall response of PD according to the investigator at the conclusion of preoperative systemic therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treatment with any anti-cancer investigational drug within 28 days prior to commencing study treatment Trastuzumab Emtansine—F. Hoffmann-La Roche Ltd 43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History of other malignancy within the last 5 years except for appropriately treated CIS of the cervix, non-melanoma skin carcinoma, Stage I uterine cancer, or other non-breast... (As per the protocol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patients for whom radiotherapy would be recommended for breast cancer treatment but for whom it is contraindicated because of medical reasons (e.g., connective tissue disorder o... (As per the protocol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current NCI CTCAE (Version 4.0) Grade ≥ 2 peripheral neuropathy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History of exposure to the following cumulative doses of anthracyclines: Doxorubicin &gt; 240 mg/m2 Epirubicin or Liposomal Doxorubicin-Hydrochloride (Myocet®) &gt; 480 mg/m2 For othe... (As per the protocol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cardiopulmonary dysfunction as defined by any of the following: History of NCI CTCAE (Version 4.0) Grade ≥ 3 symptomatic CHF or NYHA criteria Class ≥ II Angina pectoris requirin... (As per the protocol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High-risk uncontrolled arrhythmias: i.e., atrial tachycardia with a heart rate &gt; 100/min at rest, significant ventricular arrhythmia (ventricular tachycardia) or higher-grade AV... (As per the protocol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior treatment with trastuzumab emtansine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current severe, uncontrolled systemic disease (e.g., clinically significant cardiovascular, pulmonary, or metabolic disease; wound-healing disorders; ulcers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For female patients, current pregnancy and/or lactation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Major surgical procedure unrelated to breast cancer or significant traumatic injury within approximately 28 days prior to randomization or anticipation of the need for major sur... (As per the protocol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXCL016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any known active liver disease, for example, disease due to HBV, HCV, autoimmune hepatic disorders, or sclerosing cholangitis. Patients who have positive Trastuzumab Emtansine—F... (As per the protocol)</t>
   </si>
 </sst>
 </file>
@@ -820,7 +886,7 @@
         <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -829,7 +895,7 @@
         <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16">
@@ -840,10 +906,10 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
@@ -852,7 +918,7 @@
         <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17">
@@ -863,10 +929,10 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -875,7 +941,7 @@
         <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18">
@@ -886,10 +952,10 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -912,7 +978,7 @@
         <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -922,6 +988,259 @@
       </c>
       <c r="G19" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>